<commit_message>
chore: improve bold column
</commit_message>
<xml_diff>
--- a/output/CreditReportList.xlsx
+++ b/output/CreditReportList.xlsx
@@ -138,13 +138,13 @@
     </font>
     <font>
       <b/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
     </font>
     <font>
       <sz val="12"/>
-    </font>
-    <font>
-      <b/>
     </font>
     <font>
       <sz val="10"/>
@@ -170,21 +170,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -530,159 +534,166 @@
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="20" style="1" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" ht="10" customHeight="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="B3" s="1"/>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="5" ht="10" customHeight="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" ht="10" customHeight="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" ht="10" customHeight="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" ht="10" customHeight="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" ht="10" customHeight="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" ht="10" customHeight="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" ht="10" customHeight="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" ht="10" customHeight="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" ht="10" customHeight="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" ht="10" customHeight="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="10" ht="10" customHeight="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" ht="10" customHeight="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" ht="10" customHeight="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" ht="10" customHeight="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" ht="10" customHeight="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="8" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>